<commit_message>
feat: add API routes for cafes and insights, update leaderboard to use real data
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivantai/template copy 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88A86696-91FB-C24D-BBD5-1C0FB305D0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CBCF66-DD63-4242-81F7-AB2D775BEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="5580" windowWidth="40580" windowHeight="17260" xr2:uid="{A64EEFAC-6E12-2847-B40C-3A46953A0046}"/>
+    <workbookView xWindow="27920" yWindow="5340" windowWidth="40580" windowHeight="17260" xr2:uid="{A64EEFAC-6E12-2847-B40C-3A46953A0046}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,10 +473,13 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -521,7 +524,7 @@
         <v>92</v>
       </c>
       <c r="D2">
-        <v>2450</v>
+        <v>2250</v>
       </c>
       <c r="E2">
         <v>3</v>

</xml_diff>